<commit_message>
Fix ToolMessage error and add V2 enhancements
- Fix: Corrected ToolMessage creation to include synthetic AIMessage with tool_calls
- Fix: Added uuid import for generating unique tool_call_ids
- Enhancement: Added Strategy Validation Layer to V2 roadmap
- Enhancement: Added Regional & Granular Analysis to V2 roadmap
- Improvement: Adjusted Excel column widths for better readability
</commit_message>
<xml_diff>
--- a/examples/mock_business_data.xlsx
+++ b/examples/mock_business_data.xlsx
@@ -436,6 +436,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -473,7 +480,6 @@
       <c r="B2" t="n">
         <v>120</v>
       </c>
-      <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
         <v>22.1</v>
       </c>
@@ -564,6 +570,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -591,7 +602,6 @@
       <c r="B2" t="n">
         <v>2.35</v>
       </c>
-      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -754,6 +764,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -859,6 +875,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1000,6 +1023,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="27" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">

</xml_diff>